<commit_message>
Added cargo upload functionality
Any cargo files placed in the "used-cargo-plates"
folder will be uploaded to the cargo inventory
upon page load.

TODO: allow new cargo files to be uploaded
TODO: Automate actually generating megastructures
with backend
</commit_message>
<xml_diff>
--- a/cargo_plates/sw_src007_nelson_quimby_bart_edna.xlsx
+++ b/cargo_plates/sw_src007_nelson_quimby_bart_edna.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02764c23b0b97413/Cloud_Documents/Shih_Lab_2024/Crisscross-Design/cargo_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39018F26-541E-EB43-ABDC-ED029D1D11F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="732" yWindow="732" windowWidth="20214" windowHeight="12438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
@@ -1989,13 +1989,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+    <sheetView zoomScale="176" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>520</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2390,17 +2390,17 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -2612,22 +2612,22 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -2641,13 +2641,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>520</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -3042,17 +3042,17 @@
         <v>355</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -3264,22 +3264,22 @@
         <v>359</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -3297,9 +3297,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>520</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -3694,17 +3694,17 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -3916,22 +3916,22 @@
         <v>519</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
included cnt_patterning cargo plate
</commit_message>
<xml_diff>
--- a/cargo_plates/sw_src007_nelson_quimby_bart_edna.xlsx
+++ b/cargo_plates/sw_src007_nelson_quimby_bart_edna.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02764c23b0b97413/Cloud_Documents/Shih_Lab_2024/Crisscross-Design/GUI/used-cargo-plates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stellawang/Documents/gitrepos/Crisscross-Design/cargo_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{39018F26-541E-EB43-ABDC-ED029D1D11F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A6F66BB-9351-44E6-BE43-A9A2106BF368}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1E894C-2CCA-6743-9242-5B50F438C62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46540" yWindow="-2120" windowWidth="30760" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="618">
   <si>
     <t>1</t>
   </si>
@@ -1601,6 +1601,294 @@
   </si>
   <si>
     <t>name_side_position</t>
+  </si>
+  <si>
+    <t>CCTGGCCCTCTCCAACGTCAAAGGGCGACTTGACGGGGAAAGttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>CATAAAGTGGTGAGACGGGCAACAGCTGAGAAAGCGAAAGGAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>TCTGTGGTGGCTCACAATTCCACACAACCGGTCACGCTGCGCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>ATCCGCCGGGATCCAGCGCAGTGTCACTCGCCGCTACAGGGCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>TTTTCGTCTTCAGCGGGGTCATTGCAGGTATAACGTGCTTTCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>TTTCTCCGTTGCTGATTGCCGTTCCGGCAGGAGGCCGATTAAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>GCTATTACGGTTTACCAGTCCCGGAATTGAATCCTGAGAAGTttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>GACCGTAATCTGTTGGGAAGGGCGATCGAAAAGAGTCTGTCCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>GGAAGATTGCGTCGGATTCTCCGTGGGACTTCTTTGATTAGTttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>AGACAGTCACCCCGGTTGATAATCAGAACTCAAACTATCGGCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>GGCAAGGCATAGGTAAAGATTCAAAAGGCCGCCAGCCATTGCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>AATATGCAATAGTAGTAGCATTAACATCACATTTTGACGCTCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>AGCGGATTGGCTGAATATAATGCTGTAGGCAGATTCACCAGTttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>GATAAAAACGGTCTTTACCCTGACTATTTGGCCAACAGAGATttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>TAAGAACTGCAACACTATCATAACCCTCATACGTGGCACAGAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>ACGGTGTACACTTTAATCATTGTGAATTAATGCGCGAACTGAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>ACGAAAGAGCCGAACTGACCAACTTTGACCGAACGAACCACCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>CGCCCACGCTACGTAATGCCACTACGAATCAGTATTAACACCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>TTTGCTAAAACCGATAGTTGCGCCGACAGCAGCAAATGAAAAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>CCACCCTCACAGACGTTAGTAAATGAATAATATCAAACCCTCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>ACAGTTAATTCAGGAGGTTTAGTACCGCACAGTTGAAAGGAAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>CCGCCGCCAGGGTCAGTGCCTTGAGTAAGGAGCACTAACAACttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>GAATCAAGTCCCTCAGAGCCGCCACCAGACATTTGAGGATTTttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>CCAAAGACACCATCGATAGCAGCACCGTACAACTCGTATTAAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>GAACAAAGTCAATCAATAGAAAATTCATAAAGTTTGAGTAACttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>CTTTACAGAGAAGCCCTTTTTAAGAAAACCAGAAGGAGCGGAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>AACCTCCCGTTTTTGTTTAACGTCAAAAGATGGCAATTCATCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>CATCCTAATTCCGGTATTCTAAGAACGCTTCTGAATAATGGAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>GTAGGGCTTATAGATAAGTCCTGAACAATTTGCACGTAAAACttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>ATCGCAAGAAAATTCTTACCAGTATAAAGGTTTAACGTCAGAttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>ATATATGTGATATAACTATATGTAAATGTCGGGAGAAACAATttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>TCTGTAAATTAACAATTTCATTTTTTTAATGGAAACAAGTTACAAAATCttCCTACTTCATCCATTAAATCC</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 1 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 2 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 3 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 4 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 5 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 6 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 7 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 8 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 9 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 10 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 11 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 12 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 13 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 14 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 15 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 16 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 17 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 18 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 19 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 20 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 21 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 22 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 23 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 24 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 25 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 26 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 27 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 28 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 29 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 30 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 31 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>cc6hb h5 position 32 staple with tt linker and anti-Quimby handle</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos1</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos2</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos3</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos4</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos5</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos6</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos7</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos8</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos9</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos10</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos11</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos12</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos13</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos14</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos15</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos16</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos17</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos18</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos19</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos20</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos21</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos22</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos23</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos24</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos25</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos26</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos27</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos28</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos29</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos30</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos31</t>
+  </si>
+  <si>
+    <t>antiQuimby_h5_pos32</t>
   </si>
 </sst>
 </file>
@@ -1715,10 +2003,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2010,11 +2294,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>360</v>
       </c>
@@ -2091,7 +2377,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -2144,7 +2430,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -2197,7 +2483,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2250,7 +2536,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -2303,7 +2589,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -2356,7 +2642,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2409,17 +2695,113 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>522</v>
+      </c>
+      <c r="C8" t="s">
+        <v>523</v>
+      </c>
+      <c r="D8" t="s">
+        <v>524</v>
+      </c>
+      <c r="E8" t="s">
+        <v>525</v>
+      </c>
+      <c r="F8" t="s">
+        <v>526</v>
+      </c>
+      <c r="G8" t="s">
+        <v>527</v>
+      </c>
+      <c r="H8" t="s">
+        <v>528</v>
+      </c>
+      <c r="I8" t="s">
+        <v>529</v>
+      </c>
+      <c r="J8" t="s">
+        <v>530</v>
+      </c>
+      <c r="K8" t="s">
+        <v>531</v>
+      </c>
+      <c r="L8" t="s">
+        <v>532</v>
+      </c>
+      <c r="M8" t="s">
+        <v>533</v>
+      </c>
+      <c r="N8" t="s">
+        <v>534</v>
+      </c>
+      <c r="O8" t="s">
+        <v>535</v>
+      </c>
+      <c r="P8" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" t="s">
+        <v>538</v>
+      </c>
+      <c r="C9" t="s">
+        <v>539</v>
+      </c>
+      <c r="D9" t="s">
+        <v>540</v>
+      </c>
+      <c r="E9" t="s">
+        <v>541</v>
+      </c>
+      <c r="F9" t="s">
+        <v>542</v>
+      </c>
+      <c r="G9" t="s">
+        <v>543</v>
+      </c>
+      <c r="H9" t="s">
+        <v>544</v>
+      </c>
+      <c r="I9" t="s">
+        <v>545</v>
+      </c>
+      <c r="J9" t="s">
+        <v>546</v>
+      </c>
+      <c r="K9" t="s">
+        <v>547</v>
+      </c>
+      <c r="L9" t="s">
+        <v>548</v>
+      </c>
+      <c r="M9" t="s">
+        <v>549</v>
+      </c>
+      <c r="N9" t="s">
+        <v>550</v>
+      </c>
+      <c r="O9" t="s">
+        <v>551</v>
+      </c>
+      <c r="P9" t="s">
+        <v>552</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2472,7 +2854,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -2525,7 +2907,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -2578,7 +2960,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -2631,22 +3013,22 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -2660,17 +3042,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.05078125" customWidth="1"/>
-    <col min="2" max="25" width="7.20703125" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="25" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>521</v>
       </c>
@@ -2747,7 +3129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -2808,7 +3190,7 @@
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -2869,7 +3251,7 @@
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2930,7 +3312,7 @@
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -2991,7 +3373,7 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -3052,7 +3434,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -3113,26 +3495,58 @@
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>601</v>
+      </c>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
@@ -3142,26 +3556,58 @@
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>608</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>617</v>
+      </c>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
@@ -3171,7 +3617,7 @@
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -3232,7 +3678,7 @@
       <c r="X10" s="7"/>
       <c r="Y10" s="7"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -3293,7 +3739,7 @@
       <c r="X11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -3354,7 +3800,7 @@
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -3415,7 +3861,7 @@
       <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -3444,7 +3890,7 @@
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -3473,7 +3919,7 @@
       <c r="X15" s="7"/>
       <c r="Y15" s="7"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -3502,7 +3948,7 @@
       <c r="X16" s="7"/>
       <c r="Y16" s="7"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -3541,12 +3987,12 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:F21"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>360</v>
       </c>
@@ -3623,7 +4069,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -3676,7 +4122,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -3729,7 +4175,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -3782,7 +4228,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -3835,7 +4281,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -3888,7 +4334,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -3941,17 +4387,113 @@
         <v>355</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>554</v>
+      </c>
+      <c r="C8" t="s">
+        <v>555</v>
+      </c>
+      <c r="D8" t="s">
+        <v>556</v>
+      </c>
+      <c r="E8" t="s">
+        <v>557</v>
+      </c>
+      <c r="F8" t="s">
+        <v>558</v>
+      </c>
+      <c r="G8" t="s">
+        <v>559</v>
+      </c>
+      <c r="H8" t="s">
+        <v>560</v>
+      </c>
+      <c r="I8" t="s">
+        <v>561</v>
+      </c>
+      <c r="J8" t="s">
+        <v>562</v>
+      </c>
+      <c r="K8" t="s">
+        <v>563</v>
+      </c>
+      <c r="L8" t="s">
+        <v>564</v>
+      </c>
+      <c r="M8" t="s">
+        <v>565</v>
+      </c>
+      <c r="N8" t="s">
+        <v>566</v>
+      </c>
+      <c r="O8" t="s">
+        <v>567</v>
+      </c>
+      <c r="P8" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" t="s">
+        <v>570</v>
+      </c>
+      <c r="C9" t="s">
+        <v>571</v>
+      </c>
+      <c r="D9" t="s">
+        <v>572</v>
+      </c>
+      <c r="E9" t="s">
+        <v>573</v>
+      </c>
+      <c r="F9" t="s">
+        <v>574</v>
+      </c>
+      <c r="G9" t="s">
+        <v>575</v>
+      </c>
+      <c r="H9" t="s">
+        <v>576</v>
+      </c>
+      <c r="I9" t="s">
+        <v>577</v>
+      </c>
+      <c r="J9" t="s">
+        <v>578</v>
+      </c>
+      <c r="K9" t="s">
+        <v>579</v>
+      </c>
+      <c r="L9" t="s">
+        <v>580</v>
+      </c>
+      <c r="M9" t="s">
+        <v>581</v>
+      </c>
+      <c r="N9" t="s">
+        <v>582</v>
+      </c>
+      <c r="O9" t="s">
+        <v>583</v>
+      </c>
+      <c r="P9" t="s">
+        <v>584</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -4004,7 +4546,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -4057,7 +4599,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -4110,7 +4652,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -4163,22 +4705,22 @@
         <v>359</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>